<commit_message>
fixed C7 footprint; README.md, measurements
</commit_message>
<xml_diff>
--- a/hardware/go-box-power.xlsx
+++ b/hardware/go-box-power.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30820"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="31340" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="215">
   <si>
     <t>ref</t>
   </si>
@@ -72,6 +72,9 @@
     <t>Fieldname</t>
   </si>
   <si>
+    <t>Design Decision URI</t>
+  </si>
+  <si>
     <t>BT1</t>
   </si>
   <si>
@@ -351,7 +354,7 @@
     <t>GRM21BZ71E106KE15L</t>
   </si>
   <si>
-    <t>GRM0335C1E150FA01D</t>
+    <t>GCM1885C1H150JA16D</t>
   </si>
   <si>
     <t>EEE-FP1E100AR</t>
@@ -429,7 +432,7 @@
     <t>81-GRM21BZ71E106KE5L</t>
   </si>
   <si>
-    <t>81-GRM0335C1E150FA1D</t>
+    <t>81-GCM1885C1H150J16D</t>
   </si>
   <si>
     <t>667-EEE-FP1E100AR</t>
@@ -498,7 +501,7 @@
     <t>http://www.mouser.de/ProductDetail/Murata-Electronics/GRM21BZ71E106KE15L/</t>
   </si>
   <si>
-    <t>http://www.mouser.de/ProductDetail/Murata-Electronics/GRM0335C1E150FA01D/</t>
+    <t>https://www.mouser.de/ProductDetail/Murata-Electronics/GCM1885C1H150JA16D/</t>
   </si>
   <si>
     <t>http://www.mouser.de/ProductDetail/Panasonic/EEE-FP1E100AR/</t>
@@ -586,6 +589,9 @@
   </si>
   <si>
     <t>1%</t>
+  </si>
+  <si>
+    <t>15pF/50V</t>
   </si>
   <si>
     <t>Schottky Diodes &amp; Rectifiers Vr/40V Io/3A T/R</t>
@@ -1024,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1038,8 +1044,8 @@
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.1640625" bestFit="1" customWidth="1"/>
@@ -1048,9 +1054,10 @@
     <col min="14" max="15" width="6.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="73.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1102,1648 +1109,1654 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="Q4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="N5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="M6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N6" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O6" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>214</v>
+      </c>
+      <c r="R6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="Q7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="Q8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="M9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O9" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L11" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="M11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="N11" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O11" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N12" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N13" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O13" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N14" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O14" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N15" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O15" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N16" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O16" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q16" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O17" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L18" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="M18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N18" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O18" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q18" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O19" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L20" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M20" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="N20" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O20" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q20" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L21" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="M21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O21" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G22" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L22" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N22" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O22" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N23" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q23" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N24" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O24" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N25" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O25" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q25" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N26" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O26" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q26" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L27" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q27" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L28" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="M28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N28" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O28" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q28" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L29" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N29" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O29" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q29" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L30" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="M30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N30" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O30" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q30" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N31" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O31" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q31" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F32" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L32" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="M32" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="N32" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="O32" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="P32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q32" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>